<commit_message>
Updated land coverage data
</commit_message>
<xml_diff>
--- a/InputData/land/CSpULApYbP/CO2 Sequestered per Unit Land Area per Year by Pol.xlsx
+++ b/InputData/land/CSpULApYbP/CO2 Sequestered per Unit Land Area per Year by Pol.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anaxolt/Google Drive/2021/D.Development/TARGET_eps-us-3.2.1/InputData/land/CSpULApYbP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tfranc03/Downloads/Model_ICM&amp;CPL_260824/InputData/land/CSpULApYbP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6005C8A1-8F29-1B41-85EF-7B971A2E2A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D3C6FB-6F34-524B-8FEC-AF8B4CC1C1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11540" yWindow="4140" windowWidth="18840" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Carbon capture" sheetId="7" r:id="rId2"/>
     <sheet name="Calculations" sheetId="8" r:id="rId3"/>
-    <sheet name="CSpULApYbP" sheetId="3" r:id="rId4"/>
+    <sheet name="CSpULApYbP-old" sheetId="3" r:id="rId4"/>
+    <sheet name="CSpULApYbP" sheetId="9" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="acres_per_hectare">#REF!</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>CSpULApYbP CO2 Sequestered per Unit Land Area per Year by Policy</t>
   </si>
@@ -161,6 +162,9 @@
   </si>
   <si>
     <t>Mitigation action considered over a 20 year period (2010-2030)</t>
+  </si>
+  <si>
+    <t>added a new sheet to include numbers that ICM has from their experts and scenarios.</t>
   </si>
 </sst>
 </file>
@@ -335,7 +339,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -345,7 +349,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -366,18 +369,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -386,18 +397,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Body: normal cell" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -489,7 +489,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="About"/>
@@ -514,7 +514,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="About"/>
@@ -571,9 +571,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -611,9 +611,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -646,26 +646,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -698,26 +681,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -891,10 +857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A15" sqref="A15:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -912,13 +878,13 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
@@ -936,7 +902,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -958,6 +924,14 @@
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="25">
+        <v>45531</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -965,6 +939,7 @@
     <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -996,89 +971,87 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="23"/>
+      <c r="F3" s="24"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <v>2030</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="18">
         <v>2030</v>
       </c>
-      <c r="F4" s="25"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="14">
         <v>6</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <v>0.42</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <v>0.65</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>4.2</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>0.31</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>0.33</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="25"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="H7" s="17" t="s">
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="H7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="16">
         <v>1000000000</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="13">
         <v>1000</v>
       </c>
       <c r="J8" t="s">
@@ -1086,10 +1059,10 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9" s="13">
         <v>1000</v>
       </c>
       <c r="J9" t="s">
@@ -1097,21 +1070,21 @@
       </c>
     </row>
     <row r="10" spans="2:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="11" t="s">
+      <c r="C10" s="23"/>
+      <c r="D10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="H10" s="14" t="s">
+      <c r="F10" s="24"/>
+      <c r="H10" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="13">
         <v>2.4700000000000002</v>
       </c>
       <c r="J10" t="s">
@@ -1119,56 +1092,56 @@
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="12">
         <v>2030</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="18">
         <v>2030</v>
       </c>
-      <c r="F11" s="25"/>
+      <c r="F11" s="19"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="14">
         <f>D5*I10*1000000</f>
         <v>14820000</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="17">
         <f>E5*I8*I9*I7</f>
         <v>420000000000000</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="17">
         <f>F5*I8*I9*I7</f>
         <v>650000000000000</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <f>D6*I10*1000000</f>
         <v>10374000</v>
       </c>
-      <c r="E13" s="26">
+      <c r="E13" s="20">
         <f>E6*I8*I9*I7</f>
         <v>310000000000000</v>
       </c>
-      <c r="F13" s="27"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
@@ -1177,14 +1150,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1197,7 +1170,9 @@
   </sheetPr>
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1415,4 +1390,231 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41C777E-03D1-944A-BFB2-A346480E0B8C}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:AJ7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AJ1" s="2"/>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1804993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>5976480</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>